<commit_message>
feat(shiny): add shiny app beta
Besides adding shiny app, code folder was moved into shiny dir and minors bugs were fixed on functions and loadData. Also excel template was cleaned of unused fields.
</commit_message>
<xml_diff>
--- a/data/data1.xlsx
+++ b/data/data1.xlsx
@@ -5,23 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\OneDrive\Documents\UPC-DESKTOP-1S4F8E7\Tesis\tfm-repo\v0.2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\tfm-repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="107_{43A6708D-77D1-45C5-9D20-A59AED31C9E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{99E80A15-CC12-49B6-AC60-01A529C12EE0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AB01BF-ACFA-4563-9614-824F9913EC51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
   <sheets>
     <sheet name="machines" sheetId="1" r:id="rId1"/>
-    <sheet name="orders" sheetId="2" r:id="rId2"/>
-    <sheet name="jobs" sheetId="3" r:id="rId3"/>
-    <sheet name="tasks" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
+    <sheet name="jobs" sheetId="3" r:id="rId2"/>
+    <sheet name="tasks" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="duration" localSheetId="4">Sheet1!$A$1:$C$51</definedName>
+    <definedName name="duration" localSheetId="3">Sheet1!$A$1:$C$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,22 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="95">
-  <si>
-    <t>TW-01</t>
-  </si>
-  <si>
-    <t>TW-02</t>
-  </si>
-  <si>
-    <t>CNC-01</t>
-  </si>
-  <si>
-    <t>CNC-02</t>
-  </si>
-  <si>
-    <t>LC-01</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Tig welding machine 1</t>
   </si>
@@ -85,54 +69,21 @@
     <t>Laser cutter 1</t>
   </si>
   <si>
-    <t>TW</t>
-  </si>
-  <si>
-    <t>CNC</t>
-  </si>
-  <si>
-    <t>LC</t>
-  </si>
-  <si>
     <t>Job name</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Order ID</t>
-  </si>
-  <si>
-    <t>Order Name</t>
-  </si>
-  <si>
     <t>Machine ID</t>
   </si>
   <si>
-    <t>Machine Name</t>
-  </si>
-  <si>
     <t>Machine Description</t>
   </si>
   <si>
-    <t>Machine Family</t>
-  </si>
-  <si>
-    <t>Customer ID</t>
-  </si>
-  <si>
     <t>Job Release Date</t>
   </si>
   <si>
     <t>Job Due Date</t>
   </si>
   <si>
-    <t>Job Status</t>
-  </si>
-  <si>
-    <t>Job Comments</t>
-  </si>
-  <si>
     <t>Job ID</t>
   </si>
   <si>
@@ -145,15 +96,6 @@
     <t>Task Runtime</t>
   </si>
   <si>
-    <t>Predecessors Task ID</t>
-  </si>
-  <si>
-    <t>Airbus AOG bearings</t>
-  </si>
-  <si>
-    <t>Transmission Gears</t>
-  </si>
-  <si>
     <t>Rear shaft</t>
   </si>
   <si>
@@ -169,9 +111,6 @@
     <t>8H-1247 Seal support</t>
   </si>
   <si>
-    <t>Accepted</t>
-  </si>
-  <si>
     <t>Job Priority</t>
   </si>
   <si>
@@ -338,6 +277,9 @@
   </si>
   <si>
     <t>Predecessors</t>
+  </si>
+  <si>
+    <t>Predecessor Task ID</t>
   </si>
 </sst>
 </file>
@@ -696,102 +638,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF9ABDA-8F5D-4FAD-87D9-353996B99213}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="14.796875" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -800,51 +704,216 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBBB50DD-253B-4599-839F-DB4D03AE9AD6}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B56C77-D033-44C5-8405-8BE16B8FF683}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="3" width="14.19921875" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(C2+1.3*SUMIF(tasks!B$2:B$51,"= 1",tasks!D$2:D$51),0)</f>
+        <v>335</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>ROUND(C3+1.3*SUMIF(tasks!B$2:B$51,"=2",tasks!D$2:D$51),0)</f>
+        <v>242</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2">
-        <v>30150</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3">
-        <v>28014</v>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <f>ROUND(C4+1.3*SUMIF(tasks!B$2:B$51,"=3",tasks!D$2:D$51),0)</f>
+        <v>289</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>ROUND(C5+1.3*SUMIF(tasks!B$2:B$51,"=4",tasks!D$2:D$51),0)</f>
+        <v>460</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>ROUND(C6+1.3*SUMIF(tasks!B$2:B$51,"=5",tasks!D$2:D$51),0)</f>
+        <v>308</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <f>ROUND(C7+1.3*SUMIF(tasks!B$2:B$51,"=6",tasks!D$2:D$51),0)</f>
+        <v>429</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <f>ROUND(C8+1.3*SUMIF(tasks!B$2:B$51,"=7",tasks!D$2:D$51),0)</f>
+        <v>537</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <f>ROUND(C9+1.3*SUMIF(tasks!B$2:B$51,"=8",tasks!D$2:D$51),0)</f>
+        <v>320</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f>ROUND(C10+1.3*SUMIF(tasks!B$2:B$51,"=9",tasks!D$2:D$51),0)</f>
+        <v>303</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <f>ROUND(C11+1.3*SUMIF(tasks!B$2:B$51,"=10",tasks!D$2:D$51),0)</f>
+        <v>506</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -853,317 +922,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94B56C77-D033-44C5-8405-8BE16B8FF683}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="3" max="3" width="23.796875" customWidth="1"/>
-    <col min="4" max="4" width="15.796875" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>ROUND(D2+1.3*SUMIF(tasks!B$2:B$51,"= 1",tasks!D$2:D$51),0)</f>
-        <v>335</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f>ROUND(D3+1.3*SUMIF(tasks!B$2:B$51,"=2",tasks!D$2:D$51),0)</f>
-        <v>242</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <f>ROUND(D4+1.3*SUMIF(tasks!B$2:B$51,"=3",tasks!D$2:D$51),0)</f>
-        <v>289</v>
-      </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <f>ROUND(D5+1.3*SUMIF(tasks!B$2:B$51,"=4",tasks!D$2:D$51),0)</f>
-        <v>460</v>
-      </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f>ROUND(D6+1.3*SUMIF(tasks!B$2:B$51,"=5",tasks!D$2:D$51),0)</f>
-        <v>308</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <f>ROUND(D7+1.3*SUMIF(tasks!B$2:B$51,"=6",tasks!D$2:D$51),0)</f>
-        <v>429</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <f>ROUND(D8+1.3*SUMIF(tasks!B$2:B$51,"=7",tasks!D$2:D$51),0)</f>
-        <v>537</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f>ROUND(D9+1.3*SUMIF(tasks!B$2:B$51,"=8",tasks!D$2:D$51),0)</f>
-        <v>320</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <f>ROUND(D10+1.3*SUMIF(tasks!B$2:B$51,"=9",tasks!D$2:D$51),0)</f>
-        <v>303</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <f>ROUND(D11+1.3*SUMIF(tasks!B$2:B$51,"=10",tasks!D$2:D$51),0)</f>
-        <v>506</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2560049A-0C23-4326-A46D-111157680750}">
-          <x14:formula1>
-            <xm:f>orders!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B417:B1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{176CC821-1F05-48EB-9493-485681D31453}">
-          <x14:formula1>
-            <xm:f>OFFSET(orders!$A$2,0,0,COUNTA(orders!A:A)-1)</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B416</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D94EBF3-B95F-4317-AA04-8FAA7B9C9F8E}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1171,39 +934,31 @@
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.46484375" customWidth="1"/>
     <col min="4" max="4" width="12.86328125" customWidth="1"/>
-    <col min="5" max="5" width="16.19921875" customWidth="1"/>
-    <col min="6" max="6" width="10.86328125" customWidth="1"/>
-    <col min="7" max="7" width="12.53125" customWidth="1"/>
-    <col min="8" max="8" width="16.1328125" customWidth="1"/>
+    <col min="5" max="5" width="10.86328125" customWidth="1"/>
+    <col min="6" max="6" width="12.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <f>Sheet1!D2</f>
         <v>3</v>
@@ -1212,25 +967,21 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <f>Sheet1!C2</f>
         <v>53</v>
       </c>
-      <c r="E2" t="str">
-        <f>VLOOKUP(F2,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E2">
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
         <f>Sheet1!E2</f>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>Sheet1!D3</f>
         <v>1</v>
@@ -1239,21 +990,17 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="D3">
         <f>Sheet1!C3</f>
         <v>21</v>
       </c>
-      <c r="E3" t="str">
-        <f>VLOOKUP(F3,machines!A$2:D$6,4)</f>
-        <v>TW</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <f>Sheet1!D4</f>
         <v>2</v>
@@ -1262,25 +1009,21 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <f>Sheet1!C4</f>
         <v>34</v>
       </c>
-      <c r="E4" t="str">
-        <f>VLOOKUP(F4,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E4">
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
         <f>Sheet1!E4</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <f>Sheet1!D5</f>
         <v>4</v>
@@ -1289,25 +1032,21 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D5">
         <f>Sheet1!C5</f>
         <v>55</v>
       </c>
-      <c r="E5" t="str">
-        <f>VLOOKUP(F5,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E5">
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
         <f>Sheet1!E5</f>
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <f>Sheet1!D6</f>
         <v>5</v>
@@ -1316,25 +1055,21 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="D6">
         <f>Sheet1!C6</f>
         <v>95</v>
       </c>
-      <c r="E6" t="str">
-        <f>VLOOKUP(F6,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E6">
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
         <f>Sheet1!E6</f>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <f>Sheet1!D7</f>
         <v>7</v>
@@ -1343,25 +1078,21 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D7">
         <f>Sheet1!C7</f>
         <v>21</v>
       </c>
-      <c r="E7" t="str">
-        <f>VLOOKUP(F7,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E7">
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
         <f>Sheet1!E7</f>
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <f>Sheet1!D8</f>
         <v>10</v>
@@ -1370,25 +1101,21 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D8">
         <f>Sheet1!C8</f>
         <v>71</v>
       </c>
-      <c r="E8" t="str">
-        <f>VLOOKUP(F8,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E8">
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
         <f>Sheet1!E8</f>
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <f>Sheet1!D9</f>
         <v>8</v>
@@ -1397,25 +1124,21 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <f>Sheet1!C9</f>
         <v>26</v>
       </c>
-      <c r="E9" t="str">
-        <f>VLOOKUP(F9,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E9">
+        <v>3</v>
       </c>
       <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
         <f>Sheet1!E9</f>
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <f>Sheet1!D10</f>
         <v>9</v>
@@ -1424,25 +1147,21 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <f>Sheet1!C10</f>
         <v>52</v>
       </c>
-      <c r="E10" t="str">
-        <f>VLOOKUP(F10,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E10">
+        <v>4</v>
       </c>
       <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
         <f>Sheet1!E10</f>
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <f>Sheet1!D11</f>
         <v>6</v>
@@ -1451,21 +1170,17 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <f>Sheet1!C11</f>
         <v>16</v>
       </c>
-      <c r="E11" t="str">
-        <f>VLOOKUP(F11,machines!A$2:D$6,4)</f>
-        <v>LC</v>
-      </c>
-      <c r="F11">
+      <c r="E11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <f>Sheet1!D12</f>
         <v>11</v>
@@ -1474,21 +1189,17 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="D12">
         <f>Sheet1!C12</f>
         <v>12</v>
       </c>
-      <c r="E12" t="str">
-        <f>VLOOKUP(F12,machines!A$2:D$6,4)</f>
-        <v>TW</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <f>Sheet1!D13</f>
         <v>14</v>
@@ -1497,25 +1208,21 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <f>Sheet1!C13</f>
         <v>42</v>
       </c>
-      <c r="E13" t="str">
-        <f>VLOOKUP(F13,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E13">
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>2</v>
-      </c>
-      <c r="G13">
         <f>Sheet1!E13</f>
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <f>Sheet1!D14</f>
         <v>12</v>
@@ -1524,25 +1231,21 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <f>Sheet1!C14</f>
         <v>31</v>
       </c>
-      <c r="E14" t="str">
-        <f>VLOOKUP(F14,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E14">
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>3</v>
-      </c>
-      <c r="G14">
         <f>Sheet1!E14</f>
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <f>Sheet1!D15</f>
         <v>13</v>
@@ -1551,25 +1254,21 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D15">
         <f>Sheet1!C15</f>
         <v>39</v>
       </c>
-      <c r="E15" t="str">
-        <f>VLOOKUP(F15,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E15">
+        <v>4</v>
       </c>
       <c r="F15">
-        <v>4</v>
-      </c>
-      <c r="G15">
         <f>Sheet1!E15</f>
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <f>Sheet1!D16</f>
         <v>15</v>
@@ -1578,25 +1277,21 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <f>Sheet1!C16</f>
         <v>98</v>
       </c>
-      <c r="E16" t="str">
-        <f>VLOOKUP(F16,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E16">
+        <v>5</v>
       </c>
       <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16">
         <f>Sheet1!E16</f>
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <f>Sheet1!D17</f>
         <v>16</v>
@@ -1605,21 +1300,17 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D17">
         <f>Sheet1!C17</f>
         <v>55</v>
       </c>
-      <c r="E17" t="str">
-        <f>VLOOKUP(F17,machines!A$2:D$6,4)</f>
-        <v>TW</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <f>Sheet1!D18</f>
         <v>18</v>
@@ -1628,25 +1319,21 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="D18">
         <f>Sheet1!C18</f>
         <v>77</v>
       </c>
-      <c r="E18" t="str">
-        <f>VLOOKUP(F18,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E18">
+        <v>2</v>
       </c>
       <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
         <f>Sheet1!E18</f>
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <f>Sheet1!D19</f>
         <v>17</v>
@@ -1655,25 +1342,21 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <f>Sheet1!C19</f>
         <v>66</v>
       </c>
-      <c r="E19" t="str">
-        <f>VLOOKUP(F19,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E19">
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>3</v>
-      </c>
-      <c r="G19">
         <f>Sheet1!E19</f>
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <f>Sheet1!D20</f>
         <v>19</v>
@@ -1682,25 +1365,21 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="D20">
         <f>Sheet1!C20</f>
         <v>77</v>
       </c>
-      <c r="E20" t="str">
-        <f>VLOOKUP(F20,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E20">
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>4</v>
-      </c>
-      <c r="G20">
         <f>Sheet1!E20</f>
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <f>Sheet1!D21</f>
         <v>20</v>
@@ -1709,25 +1388,21 @@
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D21">
         <f>Sheet1!C21</f>
         <v>79</v>
       </c>
-      <c r="E21" t="str">
-        <f>VLOOKUP(F21,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E21">
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>5</v>
-      </c>
-      <c r="G21">
         <f>Sheet1!E21</f>
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <f>Sheet1!D22</f>
         <v>25</v>
@@ -1736,25 +1411,21 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D22">
         <f>Sheet1!C22</f>
         <v>83</v>
       </c>
-      <c r="E22" t="str">
-        <f>VLOOKUP(F22,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E22">
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
         <f>Sheet1!E22</f>
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <f>Sheet1!D23</f>
         <v>21</v>
@@ -1763,21 +1434,17 @@
         <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="D23">
         <f>Sheet1!C23</f>
         <v>19</v>
       </c>
-      <c r="E23" t="str">
-        <f>VLOOKUP(F23,machines!A$2:D$6,4)</f>
-        <v>TW</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <f>Sheet1!D24</f>
         <v>24</v>
@@ -1786,25 +1453,21 @@
         <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="D24">
         <f>Sheet1!C24</f>
         <v>64</v>
       </c>
-      <c r="E24" t="str">
-        <f>VLOOKUP(F24,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E24">
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>3</v>
-      </c>
-      <c r="G24">
         <f>Sheet1!E24</f>
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <f>Sheet1!D25</f>
         <v>22</v>
@@ -1813,25 +1476,21 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="D25">
         <f>Sheet1!C25</f>
         <v>34</v>
       </c>
-      <c r="E25" t="str">
-        <f>VLOOKUP(F25,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E25">
+        <v>4</v>
       </c>
       <c r="F25">
-        <v>4</v>
-      </c>
-      <c r="G25">
         <f>Sheet1!E25</f>
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
         <f>Sheet1!D26</f>
         <v>23</v>
@@ -1840,25 +1499,21 @@
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D26">
         <f>Sheet1!C26</f>
         <v>37</v>
       </c>
-      <c r="E26" t="str">
-        <f>VLOOKUP(F26,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E26">
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>5</v>
-      </c>
-      <c r="G26">
         <f>Sheet1!E26</f>
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <f>Sheet1!D27</f>
         <v>30</v>
@@ -1867,25 +1522,21 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="D27">
         <f>Sheet1!C27</f>
         <v>92</v>
       </c>
-      <c r="E27" t="str">
-        <f>VLOOKUP(F27,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E27">
+        <v>1</v>
       </c>
       <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
         <f>Sheet1!E27</f>
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <f>Sheet1!D28</f>
         <v>27</v>
@@ -1894,25 +1545,21 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="D28">
         <f>Sheet1!C28</f>
         <v>54</v>
       </c>
-      <c r="E28" t="str">
-        <f>VLOOKUP(F28,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E28">
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>2</v>
-      </c>
-      <c r="G28">
         <f>Sheet1!E28</f>
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
         <f>Sheet1!D29</f>
         <v>26</v>
@@ -1921,21 +1568,17 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="D29">
         <f>Sheet1!C29</f>
         <v>43</v>
       </c>
-      <c r="E29" t="str">
-        <f>VLOOKUP(F29,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
-      </c>
-      <c r="F29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
         <f>Sheet1!D30</f>
         <v>28</v>
@@ -1944,25 +1587,21 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D30">
         <f>Sheet1!C30</f>
         <v>62</v>
       </c>
-      <c r="E30" t="str">
-        <f>VLOOKUP(F30,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E30">
+        <v>4</v>
       </c>
       <c r="F30">
-        <v>4</v>
-      </c>
-      <c r="G30">
         <f>Sheet1!E30</f>
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <f>Sheet1!D31</f>
         <v>29</v>
@@ -1971,25 +1610,21 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D31">
         <f>Sheet1!C31</f>
         <v>79</v>
       </c>
-      <c r="E31" t="str">
-        <f>VLOOKUP(F31,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E31">
+        <v>5</v>
       </c>
       <c r="F31">
-        <v>5</v>
-      </c>
-      <c r="G31">
         <f>Sheet1!E31</f>
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <f>Sheet1!D32</f>
         <v>35</v>
@@ -1998,25 +1633,21 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="D32">
         <f>Sheet1!C32</f>
         <v>93</v>
       </c>
-      <c r="E32" t="str">
-        <f>VLOOKUP(F32,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E32">
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>1</v>
-      </c>
-      <c r="G32">
         <f>Sheet1!E32</f>
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <f>Sheet1!D33</f>
         <v>33</v>
@@ -2025,25 +1656,21 @@
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D33">
         <f>Sheet1!C33</f>
         <v>87</v>
       </c>
-      <c r="E33" t="str">
-        <f>VLOOKUP(F33,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E33">
+        <v>2</v>
       </c>
       <c r="F33">
-        <v>2</v>
-      </c>
-      <c r="G33">
         <f>Sheet1!E33</f>
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <f>Sheet1!D34</f>
         <v>34</v>
@@ -2052,25 +1679,21 @@
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="D34">
         <f>Sheet1!C34</f>
         <v>87</v>
       </c>
-      <c r="E34" t="str">
-        <f>VLOOKUP(F34,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E34">
+        <v>3</v>
       </c>
       <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="G34">
         <f>Sheet1!E34</f>
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <f>Sheet1!D35</f>
         <v>31</v>
@@ -2079,21 +1702,17 @@
         <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="D35">
         <f>Sheet1!C35</f>
         <v>69</v>
       </c>
-      <c r="E35" t="str">
-        <f>VLOOKUP(F35,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
-      </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
         <f>Sheet1!D36</f>
         <v>32</v>
@@ -2102,25 +1721,21 @@
         <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D36">
         <f>Sheet1!C36</f>
         <v>77</v>
       </c>
-      <c r="E36" t="str">
-        <f>VLOOKUP(F36,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E36">
+        <v>5</v>
       </c>
       <c r="F36">
-        <v>5</v>
-      </c>
-      <c r="G36">
         <f>Sheet1!E36</f>
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <f>Sheet1!D37</f>
         <v>39</v>
@@ -2129,25 +1744,21 @@
         <v>8</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D37">
         <f>Sheet1!C37</f>
         <v>60</v>
       </c>
-      <c r="E37" t="str">
-        <f>VLOOKUP(F37,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E37">
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37">
         <f>Sheet1!E37</f>
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <f>Sheet1!D38</f>
         <v>38</v>
@@ -2156,25 +1767,21 @@
         <v>8</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="D38">
         <f>Sheet1!C38</f>
         <v>41</v>
       </c>
-      <c r="E38" t="str">
-        <f>VLOOKUP(F38,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E38">
+        <v>2</v>
       </c>
       <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="G38">
         <f>Sheet1!E38</f>
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <f>Sheet1!D39</f>
         <v>37</v>
@@ -2183,25 +1790,21 @@
         <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D39">
         <f>Sheet1!C39</f>
         <v>38</v>
       </c>
-      <c r="E39" t="str">
-        <f>VLOOKUP(F39,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E39">
+        <v>3</v>
       </c>
       <c r="F39">
-        <v>3</v>
-      </c>
-      <c r="G39">
         <f>Sheet1!E39</f>
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <f>Sheet1!D40</f>
         <v>36</v>
@@ -2210,21 +1813,17 @@
         <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D40">
         <f>Sheet1!C40</f>
         <v>24</v>
       </c>
-      <c r="E40" t="str">
-        <f>VLOOKUP(F40,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
-      </c>
-      <c r="F40">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <f>Sheet1!D41</f>
         <v>40</v>
@@ -2233,25 +1832,21 @@
         <v>8</v>
       </c>
       <c r="C41" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="D41">
         <f>Sheet1!C41</f>
         <v>83</v>
       </c>
-      <c r="E41" t="str">
-        <f>VLOOKUP(F41,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E41">
+        <v>5</v>
       </c>
       <c r="F41">
-        <v>5</v>
-      </c>
-      <c r="G41">
         <f>Sheet1!E41</f>
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <f>Sheet1!D42</f>
         <v>43</v>
@@ -2260,25 +1855,21 @@
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="D42">
         <f>Sheet1!C42</f>
         <v>44</v>
       </c>
-      <c r="E42" t="str">
-        <f>VLOOKUP(F42,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E42">
+        <v>1</v>
       </c>
       <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
         <f>Sheet1!E42</f>
         <v>42</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <f>Sheet1!D43</f>
         <v>44</v>
@@ -2287,25 +1878,21 @@
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D43">
         <f>Sheet1!C43</f>
         <v>49</v>
       </c>
-      <c r="E43" t="str">
-        <f>VLOOKUP(F43,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E43">
+        <v>2</v>
       </c>
       <c r="F43">
-        <v>2</v>
-      </c>
-      <c r="G43">
         <f>Sheet1!E43</f>
         <v>43</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
         <f>Sheet1!D44</f>
         <v>45</v>
@@ -2314,25 +1901,21 @@
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D44">
         <f>Sheet1!C44</f>
         <v>98</v>
       </c>
-      <c r="E44" t="str">
-        <f>VLOOKUP(F44,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E44">
+        <v>3</v>
       </c>
       <c r="F44">
-        <v>3</v>
-      </c>
-      <c r="G44">
         <f>Sheet1!E44</f>
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
         <f>Sheet1!D45</f>
         <v>41</v>
@@ -2341,21 +1924,17 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D45">
         <f>Sheet1!C45</f>
         <v>17</v>
       </c>
-      <c r="E45" t="str">
-        <f>VLOOKUP(F45,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
-      </c>
-      <c r="F45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <f>Sheet1!D46</f>
         <v>42</v>
@@ -2364,25 +1943,21 @@
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D46">
         <f>Sheet1!C46</f>
         <v>25</v>
       </c>
-      <c r="E46" t="str">
-        <f>VLOOKUP(F46,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E46">
+        <v>5</v>
       </c>
       <c r="F46">
-        <v>5</v>
-      </c>
-      <c r="G46">
         <f>Sheet1!E46</f>
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <f>Sheet1!D47</f>
         <v>50</v>
@@ -2391,25 +1966,21 @@
         <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D47">
         <f>Sheet1!C47</f>
         <v>96</v>
       </c>
-      <c r="E47" t="str">
-        <f>VLOOKUP(F47,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E47">
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>1</v>
-      </c>
-      <c r="G47">
         <f>Sheet1!E47</f>
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
         <f>Sheet1!D48</f>
         <v>47</v>
@@ -2418,25 +1989,21 @@
         <v>10</v>
       </c>
       <c r="C48" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="D48">
         <f>Sheet1!C48</f>
         <v>75</v>
       </c>
-      <c r="E48" t="str">
-        <f>VLOOKUP(F48,machines!A$2:D$6,4)</f>
-        <v>TW</v>
+      <c r="E48">
+        <v>2</v>
       </c>
       <c r="F48">
-        <v>2</v>
-      </c>
-      <c r="G48">
         <f>Sheet1!E48</f>
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
         <f>Sheet1!D49</f>
         <v>46</v>
@@ -2445,21 +2012,17 @@
         <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D49">
         <f>Sheet1!C49</f>
         <v>43</v>
       </c>
-      <c r="E49" t="str">
-        <f>VLOOKUP(F49,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
-      </c>
-      <c r="F49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
         <f>Sheet1!D50</f>
         <v>49</v>
@@ -2468,25 +2031,21 @@
         <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="D50">
         <f>Sheet1!C50</f>
         <v>79</v>
       </c>
-      <c r="E50" t="str">
-        <f>VLOOKUP(F50,machines!A$2:D$6,4)</f>
-        <v>CNC</v>
+      <c r="E50">
+        <v>4</v>
       </c>
       <c r="F50">
-        <v>4</v>
-      </c>
-      <c r="G50">
         <f>Sheet1!E50</f>
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
         <f>Sheet1!D51</f>
         <v>48</v>
@@ -2495,25 +2054,22 @@
         <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="D51">
         <v>96</v>
       </c>
-      <c r="E51" t="str">
-        <f>VLOOKUP(F51,machines!A$2:D$6,4)</f>
-        <v>LC</v>
+      <c r="E51">
+        <v>5</v>
       </c>
       <c r="F51">
-        <v>5</v>
-      </c>
-      <c r="G51">
         <f>Sheet1!E51</f>
         <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -2521,7 +2077,7 @@
           <x14:formula1>
             <xm:f>machines!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F51</xm:sqref>
+          <xm:sqref>E2:E51</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B06DC037-BB93-4972-9EA3-B930CC649231}">
           <x14:formula1>
@@ -2535,7 +2091,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4822E5-CEBD-4040-805C-BEFEBD2AFACE}">
   <dimension ref="A1:E51"/>
   <sheetViews>
@@ -2552,19 +2108,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="E1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
@@ -3396,7 +2952,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25361361-45DB-4274-ADA1-4D75F158CC5D}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
feat(solver): handling jobs with less tasks than machines
</commit_message>
<xml_diff>
--- a/data/data1.xlsx
+++ b/data/data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samue\Desktop\tfm-repo\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AB01BF-ACFA-4563-9614-824F9913EC51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2E0D34-37EE-48F1-AD9C-91CF1BA2460B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{6639CBF0-1A6E-437C-903B-D5B18B74404F}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Tig welding machine 1</t>
   </si>
@@ -145,12 +145,6 @@
   </si>
   <si>
     <t>J2 Task 3</t>
-  </si>
-  <si>
-    <t>J2 Task 4</t>
-  </si>
-  <si>
-    <t>J2 Task 5</t>
   </si>
   <si>
     <t>J3 Task 1</t>
@@ -286,10 +280,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -747,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>ROUND(C2+1.3*SUMIF(tasks!B$2:B$51,"= 1",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C2+1.3*SUMIF(tasks!B$2:B$49,"= 1",tasks!D$2:D$49),0)</f>
         <v>335</v>
       </c>
       <c r="E2">
@@ -765,8 +765,8 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>ROUND(C3+1.3*SUMIF(tasks!B$2:B$51,"=2",tasks!D$2:D$51),0)</f>
-        <v>242</v>
+        <f>ROUND(C3+1.3*SUMIF(tasks!B$2:B$49,"=2",tasks!D$2:D$49),0)</f>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>ROUND(C4+1.3*SUMIF(tasks!B$2:B$51,"=3",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C4+1.3*SUMIF(tasks!B$2:B$49,"=3",tasks!D$2:D$49),0)</f>
         <v>289</v>
       </c>
       <c r="E4">
@@ -801,7 +801,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>ROUND(C5+1.3*SUMIF(tasks!B$2:B$51,"=4",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C5+1.3*SUMIF(tasks!B$2:B$49,"=4",tasks!D$2:D$49),0)</f>
         <v>460</v>
       </c>
       <c r="E5">
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>ROUND(C6+1.3*SUMIF(tasks!B$2:B$51,"=5",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C6+1.3*SUMIF(tasks!B$2:B$49,"=5",tasks!D$2:D$49),0)</f>
         <v>308</v>
       </c>
       <c r="E6">
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>ROUND(C7+1.3*SUMIF(tasks!B$2:B$51,"=6",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C7+1.3*SUMIF(tasks!B$2:B$49,"=6",tasks!D$2:D$49),0)</f>
         <v>429</v>
       </c>
       <c r="E7">
@@ -855,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>ROUND(C8+1.3*SUMIF(tasks!B$2:B$51,"=7",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C8+1.3*SUMIF(tasks!B$2:B$49,"=7",tasks!D$2:D$49),0)</f>
         <v>537</v>
       </c>
       <c r="E8">
@@ -873,7 +873,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <f>ROUND(C9+1.3*SUMIF(tasks!B$2:B$51,"=8",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C9+1.3*SUMIF(tasks!B$2:B$49,"=8",tasks!D$2:D$49),0)</f>
         <v>320</v>
       </c>
       <c r="E9">
@@ -891,7 +891,7 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <f>ROUND(C10+1.3*SUMIF(tasks!B$2:B$51,"=9",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C10+1.3*SUMIF(tasks!B$2:B$49,"=9",tasks!D$2:D$49),0)</f>
         <v>303</v>
       </c>
       <c r="E10">
@@ -909,7 +909,7 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <f>ROUND(C11+1.3*SUMIF(tasks!B$2:B$51,"=10",tasks!D$2:D$51),0)</f>
+        <f>ROUND(C11+1.3*SUMIF(tasks!B$2:B$49,"=10",tasks!D$2:D$49),0)</f>
         <v>506</v>
       </c>
       <c r="E11">
@@ -923,10 +923,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D94EBF3-B95F-4317-AA04-8FAA7B9C9F8E}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -955,13 +955,13 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
-        <f>Sheet1!D2</f>
-        <v>3</v>
+        <f>Sheet1!D3</f>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -970,57 +970,57 @@
         <v>23</v>
       </c>
       <c r="D2">
+        <f>Sheet1!C3</f>
+        <v>21</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <f>Sheet1!D4</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <f>Sheet1!C4</f>
+        <v>34</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <f>Sheet1!E4</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <f>Sheet1!D2</f>
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
         <f>Sheet1!C2</f>
         <v>53</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <f>Sheet1!E2</f>
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <f>Sheet1!D3</f>
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3">
-        <f>Sheet1!C3</f>
-        <v>21</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <f>Sheet1!D4</f>
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <f>Sheet1!C4</f>
-        <v>34</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <f>Sheet1!E4</f>
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1071,48 +1071,44 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
+        <f>Sheet1!D11</f>
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <f>Sheet1!C11</f>
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8">
         <f>Sheet1!D7</f>
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
         <f>Sheet1!C7</f>
         <v>21</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <f>Sheet1!E7</f>
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <f>Sheet1!D8</f>
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8">
-        <f>Sheet1!C8</f>
-        <v>71</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <f>Sheet1!E8</f>
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1140,50 +1136,50 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
-        <f>Sheet1!D10</f>
-        <v>9</v>
+        <f>Sheet1!D12</f>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10">
-        <f>Sheet1!C10</f>
-        <v>52</v>
+        <f>Sheet1!C12</f>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>4</v>
-      </c>
-      <c r="F10">
-        <f>Sheet1!E10</f>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
-        <f>Sheet1!D11</f>
-        <v>6</v>
+        <f>Sheet1!D14</f>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
       </c>
       <c r="D11">
-        <f>Sheet1!C11</f>
-        <v>16</v>
+        <f>Sheet1!C14</f>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f>Sheet1!E14</f>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
-        <f>Sheet1!D12</f>
-        <v>11</v>
+        <f>Sheet1!D15</f>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1192,11 +1188,15 @@
         <v>33</v>
       </c>
       <c r="D12">
-        <f>Sheet1!C12</f>
+        <f>Sheet1!C15</f>
+        <v>39</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <f>Sheet1!E15</f>
         <v>12</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1224,8 +1224,8 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
-        <f>Sheet1!D14</f>
-        <v>12</v>
+        <f>Sheet1!D16</f>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -1234,67 +1234,63 @@
         <v>35</v>
       </c>
       <c r="D14">
-        <f>Sheet1!C14</f>
-        <v>31</v>
+        <f>Sheet1!C16</f>
+        <v>98</v>
       </c>
       <c r="E14">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F14">
-        <f>Sheet1!E14</f>
-        <v>11</v>
+        <f>Sheet1!E16</f>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
-        <f>Sheet1!D15</f>
-        <v>13</v>
+        <f>Sheet1!D17</f>
+        <v>16</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
       </c>
       <c r="D15">
-        <f>Sheet1!C15</f>
-        <v>39</v>
+        <f>Sheet1!C17</f>
+        <v>55</v>
       </c>
       <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
-        <f>Sheet1!E15</f>
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
-        <f>Sheet1!D16</f>
-        <v>15</v>
+        <f>Sheet1!D19</f>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
       </c>
       <c r="D16">
-        <f>Sheet1!C16</f>
-        <v>98</v>
+        <f>Sheet1!C19</f>
+        <v>66</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <f>Sheet1!E16</f>
-        <v>14</v>
+        <f>Sheet1!E19</f>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
-        <f>Sheet1!D17</f>
-        <v>16</v>
+        <f>Sheet1!D18</f>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1303,17 +1299,21 @@
         <v>38</v>
       </c>
       <c r="D17">
-        <f>Sheet1!C17</f>
-        <v>55</v>
+        <f>Sheet1!C18</f>
+        <v>77</v>
       </c>
       <c r="E17">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <f>Sheet1!E18</f>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
-        <f>Sheet1!D18</f>
-        <v>18</v>
+        <f>Sheet1!D20</f>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -1322,21 +1322,21 @@
         <v>39</v>
       </c>
       <c r="D18">
-        <f>Sheet1!C18</f>
+        <f>Sheet1!C20</f>
         <v>77</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F18">
-        <f>Sheet1!E18</f>
-        <v>17</v>
+        <f>Sheet1!E20</f>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
-        <f>Sheet1!D19</f>
-        <v>17</v>
+        <f>Sheet1!D21</f>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -1345,368 +1345,364 @@
         <v>40</v>
       </c>
       <c r="D19">
-        <f>Sheet1!C19</f>
-        <v>66</v>
+        <f>Sheet1!C21</f>
+        <v>79</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <f>Sheet1!E19</f>
-        <v>16</v>
+        <f>Sheet1!E21</f>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
-        <f>Sheet1!D20</f>
-        <v>19</v>
+        <f>Sheet1!D23</f>
+        <v>21</v>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
       </c>
       <c r="D20">
-        <f>Sheet1!C20</f>
-        <v>77</v>
+        <f>Sheet1!C23</f>
+        <v>19</v>
       </c>
       <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="F20">
-        <f>Sheet1!E20</f>
-        <v>18</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
-        <f>Sheet1!D21</f>
-        <v>20</v>
+        <f>Sheet1!D25</f>
+        <v>22</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
         <v>42</v>
       </c>
       <c r="D21">
-        <f>Sheet1!C21</f>
-        <v>79</v>
+        <f>Sheet1!C25</f>
+        <v>34</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21">
-        <f>Sheet1!E21</f>
-        <v>19</v>
+        <f>Sheet1!E25</f>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
+        <f>Sheet1!D26</f>
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22">
+        <f>Sheet1!C26</f>
+        <v>37</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <f>Sheet1!E26</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A23">
+        <f>Sheet1!D24</f>
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23">
+        <f>Sheet1!C24</f>
+        <v>64</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <f>Sheet1!E24</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A24">
         <f>Sheet1!D22</f>
         <v>25</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22">
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24">
         <f>Sheet1!C22</f>
         <v>83</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <f>Sheet1!E22</f>
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23">
-        <f>Sheet1!D23</f>
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23">
-        <f>Sheet1!C23</f>
-        <v>19</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A24">
-        <f>Sheet1!D24</f>
-        <v>24</v>
-      </c>
-      <c r="B24">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24">
-        <f>Sheet1!C24</f>
-        <v>64</v>
-      </c>
-      <c r="E24">
-        <v>3</v>
-      </c>
-      <c r="F24">
-        <f>Sheet1!E24</f>
-        <v>23</v>
-      </c>
-    </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
-        <f>Sheet1!D25</f>
-        <v>22</v>
+        <f>Sheet1!D29</f>
+        <v>26</v>
       </c>
       <c r="B25">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
       </c>
       <c r="D25">
-        <f>Sheet1!C25</f>
-        <v>34</v>
+        <f>Sheet1!C29</f>
+        <v>43</v>
       </c>
       <c r="E25">
-        <v>4</v>
-      </c>
-      <c r="F25">
-        <f>Sheet1!E25</f>
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
-        <f>Sheet1!D26</f>
-        <v>23</v>
+        <f>Sheet1!D28</f>
+        <v>27</v>
       </c>
       <c r="B26">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>47</v>
       </c>
       <c r="D26">
-        <f>Sheet1!C26</f>
-        <v>37</v>
+        <f>Sheet1!C28</f>
+        <v>54</v>
       </c>
       <c r="E26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F26">
-        <f>Sheet1!E26</f>
-        <v>22</v>
+        <f>Sheet1!E28</f>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
+        <f>Sheet1!D30</f>
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27">
+        <f>Sheet1!C30</f>
+        <v>62</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <f>Sheet1!E30</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A28">
+        <f>Sheet1!D31</f>
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28">
+        <f>Sheet1!C31</f>
+        <v>79</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <f>Sheet1!E31</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29">
         <f>Sheet1!D27</f>
         <v>30</v>
       </c>
-      <c r="B27">
+      <c r="B29">
         <v>6</v>
       </c>
-      <c r="C27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27">
+      <c r="C29" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29">
         <f>Sheet1!C27</f>
         <v>92</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
         <f>Sheet1!E27</f>
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A28">
-        <f>Sheet1!D28</f>
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28">
-        <f>Sheet1!C28</f>
-        <v>54</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
-      </c>
-      <c r="F28">
-        <f>Sheet1!E28</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A29">
-        <f>Sheet1!D29</f>
-        <v>26</v>
-      </c>
-      <c r="B29">
-        <v>6</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29">
-        <f>Sheet1!C29</f>
-        <v>43</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
-      </c>
-    </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
-        <f>Sheet1!D30</f>
-        <v>28</v>
+        <f>Sheet1!D35</f>
+        <v>31</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
         <v>51</v>
       </c>
       <c r="D30">
-        <f>Sheet1!C30</f>
-        <v>62</v>
+        <f>Sheet1!C35</f>
+        <v>69</v>
       </c>
       <c r="E30">
         <v>4</v>
-      </c>
-      <c r="F30">
-        <f>Sheet1!E30</f>
-        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
-        <f>Sheet1!D31</f>
-        <v>29</v>
+        <f>Sheet1!D36</f>
+        <v>32</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
         <v>52</v>
       </c>
       <c r="D31">
-        <f>Sheet1!C31</f>
-        <v>79</v>
+        <f>Sheet1!C36</f>
+        <v>77</v>
       </c>
       <c r="E31">
         <v>5</v>
       </c>
       <c r="F31">
-        <f>Sheet1!E31</f>
-        <v>28</v>
+        <f>Sheet1!E36</f>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
+        <f>Sheet1!D33</f>
+        <v>33</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+      <c r="D32">
+        <f>Sheet1!C33</f>
+        <v>87</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <f>Sheet1!E33</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A33">
+        <f>Sheet1!D34</f>
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33">
+        <f>Sheet1!C34</f>
+        <v>87</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <f>Sheet1!E34</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A34">
         <f>Sheet1!D32</f>
         <v>35</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>7</v>
       </c>
-      <c r="C32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32">
+      <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34">
         <f>Sheet1!C32</f>
         <v>93</v>
       </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
         <f>Sheet1!E32</f>
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33">
-        <f>Sheet1!D33</f>
-        <v>33</v>
-      </c>
-      <c r="B33">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33">
-        <f>Sheet1!C33</f>
-        <v>87</v>
-      </c>
-      <c r="E33">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <f>Sheet1!E33</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34">
-        <f>Sheet1!D34</f>
-        <v>34</v>
-      </c>
-      <c r="B34">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>55</v>
-      </c>
-      <c r="D34">
-        <f>Sheet1!C34</f>
-        <v>87</v>
-      </c>
-      <c r="E34">
-        <v>3</v>
-      </c>
-      <c r="F34">
-        <f>Sheet1!E34</f>
-        <v>33</v>
-      </c>
-    </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
-        <f>Sheet1!D35</f>
-        <v>31</v>
+        <f>Sheet1!D40</f>
+        <v>36</v>
       </c>
       <c r="B35">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C35" t="s">
         <v>56</v>
       </c>
       <c r="D35">
-        <f>Sheet1!C35</f>
-        <v>69</v>
+        <f>Sheet1!C40</f>
+        <v>24</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -1714,77 +1710,77 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
-        <f>Sheet1!D36</f>
-        <v>32</v>
+        <f>Sheet1!D39</f>
+        <v>37</v>
       </c>
       <c r="B36">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
         <v>57</v>
       </c>
       <c r="D36">
-        <f>Sheet1!C36</f>
-        <v>77</v>
+        <f>Sheet1!C39</f>
+        <v>38</v>
       </c>
       <c r="E36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F36">
-        <f>Sheet1!E36</f>
-        <v>31</v>
+        <f>Sheet1!E39</f>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
+        <f>Sheet1!D38</f>
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>58</v>
+      </c>
+      <c r="D37">
+        <f>Sheet1!C38</f>
+        <v>41</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <f>Sheet1!E38</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A38">
         <f>Sheet1!D37</f>
         <v>39</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>8</v>
       </c>
-      <c r="C37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37">
+      <c r="C38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38">
         <f>Sheet1!C37</f>
         <v>60</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38">
         <f>Sheet1!E37</f>
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38">
-        <f>Sheet1!D38</f>
-        <v>38</v>
-      </c>
-      <c r="B38">
-        <v>8</v>
-      </c>
-      <c r="C38" t="s">
-        <v>59</v>
-      </c>
-      <c r="D38">
-        <f>Sheet1!C38</f>
-        <v>41</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38">
-        <f>Sheet1!E38</f>
-        <v>37</v>
-      </c>
-    </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
-        <f>Sheet1!D39</f>
-        <v>37</v>
+        <f>Sheet1!D41</f>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>8</v>
@@ -1793,31 +1789,31 @@
         <v>60</v>
       </c>
       <c r="D39">
-        <f>Sheet1!C39</f>
-        <v>38</v>
+        <f>Sheet1!C41</f>
+        <v>83</v>
       </c>
       <c r="E39">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F39">
-        <f>Sheet1!E39</f>
-        <v>36</v>
+        <f>Sheet1!E41</f>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
-        <f>Sheet1!D40</f>
-        <v>36</v>
+        <f>Sheet1!D45</f>
+        <v>41</v>
       </c>
       <c r="B40">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
       </c>
       <c r="D40">
-        <f>Sheet1!C40</f>
-        <v>24</v>
+        <f>Sheet1!C45</f>
+        <v>17</v>
       </c>
       <c r="E40">
         <v>4</v>
@@ -1825,25 +1821,25 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
-        <f>Sheet1!D41</f>
-        <v>40</v>
+        <f>Sheet1!D46</f>
+        <v>42</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
         <v>62</v>
       </c>
       <c r="D41">
-        <f>Sheet1!C41</f>
-        <v>83</v>
+        <f>Sheet1!C46</f>
+        <v>25</v>
       </c>
       <c r="E41">
         <v>5</v>
       </c>
       <c r="F41">
-        <f>Sheet1!E41</f>
-        <v>39</v>
+        <f>Sheet1!E46</f>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -1917,157 +1913,119 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
-        <f>Sheet1!D45</f>
-        <v>41</v>
+        <f>Sheet1!D49</f>
+        <v>46</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
         <v>66</v>
       </c>
       <c r="D45">
-        <f>Sheet1!C45</f>
-        <v>17</v>
+        <f>Sheet1!C49</f>
+        <v>43</v>
       </c>
       <c r="E45">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
-        <f>Sheet1!D46</f>
-        <v>42</v>
+        <f>Sheet1!D48</f>
+        <v>47</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C46" t="s">
         <v>67</v>
       </c>
       <c r="D46">
-        <f>Sheet1!C46</f>
-        <v>25</v>
+        <f>Sheet1!C48</f>
+        <v>75</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F46">
-        <f>Sheet1!E46</f>
-        <v>41</v>
+        <f>Sheet1!E48</f>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
+        <f>Sheet1!D51</f>
+        <v>48</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47">
+        <v>96</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
+      <c r="F47">
+        <f>Sheet1!E51</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A48">
+        <f>Sheet1!D50</f>
+        <v>49</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48">
+        <f>Sheet1!C50</f>
+        <v>79</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48">
+        <f>Sheet1!E50</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A49">
         <f>Sheet1!D47</f>
         <v>50</v>
       </c>
-      <c r="B47">
+      <c r="B49">
         <v>10</v>
       </c>
-      <c r="C47" t="s">
-        <v>68</v>
-      </c>
-      <c r="D47">
+      <c r="C49" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49">
         <f>Sheet1!C47</f>
         <v>96</v>
       </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47">
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
         <f>Sheet1!E47</f>
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48">
-        <f>Sheet1!D48</f>
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>10</v>
-      </c>
-      <c r="C48" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48">
-        <f>Sheet1!C48</f>
-        <v>75</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="F48">
-        <f>Sheet1!E48</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A49">
-        <f>Sheet1!D49</f>
-        <v>46</v>
-      </c>
-      <c r="B49">
-        <v>10</v>
-      </c>
-      <c r="C49" t="s">
-        <v>70</v>
-      </c>
-      <c r="D49">
-        <f>Sheet1!C49</f>
-        <v>43</v>
-      </c>
-      <c r="E49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A50">
-        <f>Sheet1!D50</f>
-        <v>49</v>
-      </c>
-      <c r="B50">
-        <v>10</v>
-      </c>
-      <c r="C50" t="s">
-        <v>71</v>
-      </c>
-      <c r="D50">
-        <f>Sheet1!C50</f>
-        <v>79</v>
-      </c>
-      <c r="E50">
-        <v>4</v>
-      </c>
-      <c r="F50">
-        <f>Sheet1!E50</f>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A51">
-        <f>Sheet1!D51</f>
-        <v>48</v>
-      </c>
-      <c r="B51">
-        <v>10</v>
-      </c>
-      <c r="C51" t="s">
-        <v>72</v>
-      </c>
-      <c r="D51">
-        <v>96</v>
-      </c>
-      <c r="E51">
-        <v>5</v>
-      </c>
-      <c r="F51">
-        <f>Sheet1!E51</f>
-        <v>47</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F49">
+    <sortCondition ref="A1"/>
+  </sortState>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -2077,13 +2035,13 @@
           <x14:formula1>
             <xm:f>machines!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E51</xm:sqref>
+          <xm:sqref>E2:E49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B06DC037-BB93-4972-9EA3-B930CC649231}">
           <x14:formula1>
             <xm:f>OFFSET(jobs!$A$2,0,0,COUNTA(jobs!A:A)-1)</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B69</xm:sqref>
+          <xm:sqref>B2:B67</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2117,10 +2075,10 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">

</xml_diff>